<commit_message>
add new test decreasePayment
</commit_message>
<xml_diff>
--- a/doc/sample.xlsx
+++ b/doc/sample.xlsx
@@ -52,7 +52,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$руб.-419];[RED]\-#,##0.00\ [$руб.-419]"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -78,57 +78,83 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="Lucida Sans"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="Lucida Sans"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="Lucida Sans"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Lucida Sans"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -251,22 +277,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -277,7 +335,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,7 +351,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,10 +452,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L13"/>
+  <dimension ref="A2:M13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -406,12 +464,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,7 +485,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>47218.36</v>
+        <v>47778.52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,15 +529,15 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="n">
-        <f aca="false"> C2*(D3 + (D3 / ((1 + D3)^C4 - 1)))</f>
+        <f aca="false">C2*(D3 + (D3 / ((1 + D3)^C4 - 1)))</f>
         <v>17156.1394185592</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="5" t="n">
-        <f aca="false"> I2*(J3 + (J3 / ((1 + J3)^I4 - 1)))</f>
-        <v>16002.5032062243</v>
+        <f aca="false">I2*(J3 + (J3 / ((1 + J3)^I4 - 1)))</f>
+        <v>16192.3438147503</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,6 +639,10 @@
         <f aca="false">$C$5-C10</f>
         <v>16595.9863815134</v>
       </c>
+      <c r="E10" s="5" t="n">
+        <f aca="false">D10+C10</f>
+        <v>17156.1394185593</v>
+      </c>
       <c r="H10" s="7" t="n">
         <v>2</v>
       </c>
@@ -589,9 +653,13 @@
         <v>560.153037045872</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>16595.9863815134</v>
+        <v>19439.8469629541</v>
       </c>
       <c r="L10" s="3" t="n">
+        <f aca="false">20000-J10</f>
+        <v>19439.8469629541</v>
+      </c>
+      <c r="M10" s="3" t="n">
         <v>20000</v>
       </c>
     </row>
@@ -616,16 +684,17 @@
       </c>
       <c r="I11" s="3" t="n">
         <f aca="false">I10-L10</f>
-        <v>47218.3644455046</v>
+        <v>47778.5174825505</v>
       </c>
       <c r="J11" s="3" t="n">
         <f aca="false">I11*J$3</f>
-        <v>393.486370379205</v>
+        <v>398.154312354587</v>
       </c>
       <c r="K11" s="3" t="n">
         <f aca="false">I$5-J11</f>
-        <v>15609.0168358451</v>
-      </c>
+        <v>15794.1895023957</v>
+      </c>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="n">
@@ -648,15 +717,15 @@
       </c>
       <c r="I12" s="3" t="n">
         <f aca="false">I11-K11</f>
-        <v>31609.3476096595</v>
+        <v>31984.3279801548</v>
       </c>
       <c r="J12" s="3" t="n">
         <f aca="false">I12*J$3</f>
-        <v>263.411230080496</v>
+        <v>266.53606650129</v>
       </c>
       <c r="K12" s="3" t="n">
         <f aca="false">I$5-J12</f>
-        <v>15739.0919761438</v>
+        <v>15925.807748249</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,15 +749,15 @@
       </c>
       <c r="I13" s="3" t="n">
         <f aca="false">I12-K12</f>
-        <v>15870.2556335157</v>
+        <v>16058.5202319058</v>
       </c>
       <c r="J13" s="3" t="n">
         <f aca="false">I13*J$3</f>
-        <v>132.252130279298</v>
+        <v>133.821001932548</v>
       </c>
       <c r="K13" s="3" t="n">
         <f aca="false">I$5-J13</f>
-        <v>15870.251075945</v>
+        <v>16058.5228128177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>